<commit_message>
Updated conversion factor for eV in tests
</commit_message>
<xml_diff>
--- a/pmutt/tests/test_constants.xlsx
+++ b/pmutt/tests/test_constants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox (Personal)\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_development\pmutt\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDelDocuments\UDelResearch\Github\pmutt_dev\pmutt\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AD5D86-6B8C-4B02-B30B-8DF260F59294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8FE02F-360F-4B65-9118-87AD3CC28EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{AA336A12-CD5D-469F-9132-8EBAE81227A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AA336A12-CD5D-469F-9132-8EBAE81227A9}"/>
   </bookViews>
   <sheets>
     <sheet name="ans" sheetId="3" r:id="rId1"/>
@@ -81,7 +81,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1431,19 +1433,19 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>0</v>
@@ -1509,7 +1511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -1578,7 +1580,7 @@
         <v>3.1668104999999999E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -1625,7 +1627,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -1658,7 +1660,7 @@
         <v>3.1668104999999999E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>77</v>
       </c>
@@ -1671,7 +1673,7 @@
         <v>29979245800</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
@@ -1688,7 +1690,7 @@
         <v>5.4857990907000004E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>79</v>
       </c>
@@ -1705,7 +1707,7 @@
         <v>1.007276466879</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>80</v>
       </c>
@@ -1742,7 +1744,7 @@
         <v>750.06200000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -1763,7 +1765,7 @@
         <v>76.999999999999943</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -1784,7 +1786,7 @@
         <v>24.789561893699997</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>83</v>
       </c>
@@ -1808,43 +1810,43 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B12" s="2">
         <f>test_constants!B22</f>
-        <v>24177991103754.523</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24179892822261.859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="2">
         <f>test_constants!B26</f>
-        <v>1160.3609474768741</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1160.4522156008277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="2">
         <f>test_constants!B30</f>
-        <v>806.49097262328473</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>806.55440712460688</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B15" s="2">
         <f>test_constants!B34*constants!B15/constants!B17</f>
-        <v>2.5689025147068248E-39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2.5691045715871832E-39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -1853,7 +1855,7 @@
         <v>1161.4172082551468</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
@@ -1862,16 +1864,16 @@
         <v>807.22511037952791</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B18" s="2">
         <f>test_constants!B46</f>
-        <v>0.55933568955994584</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.55937968407661531</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>91</v>
       </c>
@@ -1880,7 +1882,7 @@
         <v>1.6015522831999997E-20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>92</v>
       </c>
@@ -1889,7 +1891,7 @@
         <v>24170470181145.258</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>93</v>
       </c>
@@ -1898,7 +1900,7 @@
         <v>806.24010164876324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>94</v>
       </c>
@@ -1907,7 +1909,7 @@
         <v>1.6090211175791243E-20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>95</v>
       </c>
@@ -1916,7 +1918,7 @@
         <v>24283189098000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>96</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>3.1034429993183841E-30</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>97</v>
       </c>
@@ -1934,7 +1936,7 @@
         <v>1165.4096566004534</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>98</v>
       </c>
@@ -1943,7 +1945,7 @@
         <v>173.28913505677048</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>99</v>
       </c>
@@ -1961,31 +1963,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E805CA-ACAA-4599-A8B2-1C6F37F3FD7A}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>75</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>275</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <f>h_Js/2/PI()</f>
         <v>1.0545718001391127E-34</v>
@@ -1994,7 +1996,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <f>h_kJs/2/PI()</f>
         <v>1.0545718001391128E-37</v>
@@ -2003,7 +2005,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <f>h_eVs/2/PI()</f>
         <v>6.5821195139260184E-16</v>
@@ -2012,7 +2014,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <f>h_Ehs/2/PI()</f>
         <v>2.4188843264949407E-17</v>
@@ -2021,7 +2023,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20">
         <f>h_Has/2/PI()</f>
         <v>2.4188843264949407E-17</v>
@@ -2030,18 +2032,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>298.14999999999998</v>
       </c>
@@ -2049,7 +2051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <f>A11-273.15</f>
         <v>25</v>
@@ -2058,7 +2060,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <f>(A12*9/5)+32</f>
         <v>77</v>
@@ -2067,7 +2069,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <f>A13+459.67</f>
         <v>536.67000000000007</v>
@@ -2076,17 +2078,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="8"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>106</v>
       </c>
       <c r="B16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>0.1</v>
       </c>
@@ -2094,7 +2096,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20">
         <f>1/6242000000000000000</f>
         <v>1.6020506247997438E-19</v>
@@ -2103,15 +2105,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>84</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>100</v>
       </c>
@@ -2122,27 +2124,27 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B22" s="10">
         <f>B21*constants!B15/constants!B17/h_Js</f>
-        <v>24177991103754.523</v>
+        <v>24179892822261.859</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>85</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>100</v>
       </c>
@@ -2153,29 +2155,29 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>104</v>
       </c>
       <c r="B26" s="10">
         <f>B21*constants!B15/constants!B17/kb_JK</f>
-        <v>1160.3609474768741</v>
+        <v>1160.4522156008277</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>100</v>
       </c>
@@ -2186,27 +2188,27 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B30" s="10">
         <f>B21*constants!B15/constants!B17/h_Js/c_cms</f>
-        <v>806.49097262328473</v>
+        <v>806.55440712460688</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="32" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
         <v>87</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>102</v>
       </c>
@@ -2217,7 +2219,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>100</v>
       </c>
@@ -2229,15 +2231,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="36" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>102</v>
       </c>
@@ -2248,7 +2250,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>104</v>
       </c>
@@ -2260,15 +2262,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="40" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>102</v>
       </c>
@@ -2279,7 +2281,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>109</v>
       </c>
@@ -2291,15 +2293,15 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="44" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>110</v>
       </c>
@@ -2310,28 +2312,28 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B46" s="10">
         <f>(h_eVs/2/PI())^2/2/kb_eVK/B45/constants!B17</f>
-        <v>0.55933568955994584</v>
+        <v>0.55937968407661531</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="48" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>91</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>104</v>
       </c>
@@ -2342,7 +2344,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>100</v>
       </c>
@@ -2354,15 +2356,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="52" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>92</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>104</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>102</v>
       </c>
@@ -2385,15 +2387,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="56" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
         <v>93</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="5"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>104</v>
       </c>
@@ -2404,7 +2406,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>109</v>
       </c>
@@ -2416,15 +2418,15 @@
         <v>279</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="60" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">
         <v>94</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>109</v>
       </c>
@@ -2435,7 +2437,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>100</v>
       </c>
@@ -2447,15 +2449,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="64" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A64" s="16" t="s">
         <v>95</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="5"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>109</v>
       </c>
@@ -2466,7 +2468,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>102</v>
       </c>
@@ -2478,15 +2480,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="68" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="68" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A68" s="16" t="s">
         <v>96</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="5"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>109</v>
       </c>
@@ -2497,7 +2499,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>110</v>
       </c>
@@ -2509,15 +2511,15 @@
         <v>276</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="72" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A72" s="16" t="s">
         <v>97</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="5"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>109</v>
       </c>
@@ -2528,7 +2530,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
         <v>104</v>
       </c>
@@ -2540,15 +2542,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="76" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="76" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A76" s="16" t="s">
         <v>98</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="5"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>277</v>
       </c>
@@ -2559,7 +2561,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
         <v>278</v>
       </c>
@@ -2571,15 +2573,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="80" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A80" s="16" t="s">
         <v>99</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>278</v>
       </c>
@@ -2590,7 +2592,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
         <v>277</v>
       </c>
@@ -2613,50 +2615,50 @@
   <dimension ref="A1:AH211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="12" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2664,7 +2666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2678,7 +2680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2734,7 +2736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2838,7 +2840,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2873,7 +2875,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2909,7 +2911,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -2929,7 +2931,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -2943,7 +2945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2981,7 +2983,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -3031,7 +3033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -3059,7 +3061,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -3087,14 +3089,14 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>266</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>107</v>
       </c>
@@ -3102,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>220</v>
       </c>
@@ -3110,15 +3112,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="22">
-        <v>6.242E+18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="2">
+        <v>6.2415090744607498E+18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>221</v>
       </c>
@@ -3126,7 +3128,7 @@
         <v>0.239006</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>222</v>
       </c>
@@ -3134,7 +3136,7 @@
         <v>2.3900599999999999E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>265</v>
       </c>
@@ -3142,7 +3144,7 @@
         <v>101.33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>223</v>
       </c>
@@ -3150,7 +3152,7 @@
         <v>2293710448690590</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>224</v>
       </c>
@@ -3158,14 +3160,14 @@
         <v>2293710448690590</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>267</v>
       </c>
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>225</v>
       </c>
@@ -3173,7 +3175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>226</v>
       </c>
@@ -3181,7 +3183,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>227</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>0.239006</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>228</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>2.3900599999999999E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>229</v>
       </c>
@@ -3206,7 +3208,7 @@
         <v>1.0365084685182871E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>230</v>
       </c>
@@ -3215,7 +3217,7 @@
         <v>3.808795745589036E-9</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>231</v>
       </c>
@@ -3224,7 +3226,7 @@
         <v>3.808795745589036E-9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>232</v>
       </c>
@@ -3233,7 +3235,7 @@
         <v>1.0365084685182871E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>233</v>
       </c>
@@ -3242,7 +3244,7 @@
         <v>3.808795745589036E-9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>234</v>
       </c>
@@ -3251,14 +3253,14 @@
         <v>3.808795745589036E-9</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>268</v>
       </c>
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>235</v>
       </c>
@@ -3266,7 +3268,7 @@
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>236</v>
       </c>
@@ -3274,7 +3276,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>237</v>
       </c>
@@ -3282,7 +3284,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>238</v>
       </c>
@@ -3290,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>239</v>
       </c>
@@ -3299,7 +3301,7 @@
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>240</v>
       </c>
@@ -3308,7 +3310,7 @@
         <v>2.7777777777777778E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>241</v>
       </c>
@@ -3317,7 +3319,7 @@
         <v>1.1574074074074073E-5</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>242</v>
       </c>
@@ -3326,14 +3328,14 @@
         <v>3.1688087814028947E-8</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>269</v>
       </c>
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>243</v>
       </c>
@@ -3341,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>244</v>
       </c>
@@ -3349,7 +3351,7 @@
         <v>6.0221408599999999E+23</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>245</v>
       </c>
@@ -3357,7 +3359,7 @@
         <v>6.0221408599999999E+23</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>246</v>
       </c>
@@ -3365,17 +3367,17 @@
         <v>6.0221408599999999E+23</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="24"/>
       <c r="B51" s="25"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="26" t="s">
         <v>270</v>
       </c>
       <c r="B52" s="27"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>247</v>
       </c>
@@ -3383,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>248</v>
       </c>
@@ -3391,7 +3393,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>249</v>
       </c>
@@ -3399,7 +3401,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>250</v>
       </c>
@@ -3407,7 +3409,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>251</v>
       </c>
@@ -3415,7 +3417,7 @@
         <v>39.370100000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>252</v>
       </c>
@@ -3423,7 +3425,7 @@
         <v>3.28084</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>253</v>
       </c>
@@ -3432,7 +3434,7 @@
         <v>6.2137119223733392E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>254</v>
       </c>
@@ -3440,16 +3442,16 @@
         <v>10000000000</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B62" s="27"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>255</v>
       </c>
@@ -3457,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>256</v>
       </c>
@@ -3465,7 +3467,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>257</v>
       </c>
@@ -3473,7 +3475,7 @@
         <v>1E+20</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>258</v>
       </c>
@@ -3481,7 +3483,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>259</v>
       </c>
@@ -3489,7 +3491,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>260</v>
       </c>
@@ -3497,14 +3499,14 @@
         <v>10.7639</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>272</v>
       </c>
       <c r="B70" s="5"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>42</v>
       </c>
@@ -3512,7 +3514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>43</v>
       </c>
@@ -3520,7 +3522,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>44</v>
       </c>
@@ -3528,7 +3530,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>45</v>
       </c>
@@ -3536,7 +3538,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>261</v>
       </c>
@@ -3544,7 +3546,7 @@
         <v>61023.7</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>262</v>
       </c>
@@ -3552,14 +3554,14 @@
         <v>35.314700000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>273</v>
       </c>
       <c r="B78" s="5"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>69</v>
       </c>
@@ -3567,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>70</v>
       </c>
@@ -3575,7 +3577,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>71</v>
       </c>
@@ -3583,7 +3585,7 @@
         <v>6.0219999999999999E+26</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
         <v>263</v>
       </c>
@@ -3591,14 +3593,14 @@
         <v>2.2046199999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>274</v>
       </c>
       <c r="B84" s="5"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>12</v>
       </c>
@@ -3606,7 +3608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>13</v>
       </c>
@@ -3614,7 +3616,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>111</v>
       </c>
@@ -3622,7 +3624,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>11</v>
       </c>
@@ -3630,7 +3632,7 @@
         <v>9.8692300000000007E-6</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>10</v>
       </c>
@@ -3638,7 +3640,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>15</v>
       </c>
@@ -3646,7 +3648,7 @@
         <v>7.5006200000000004E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>264</v>
       </c>
@@ -3654,7 +3656,7 @@
         <v>7.5006200000000004E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
         <v>14</v>
       </c>
@@ -3662,14 +3664,14 @@
         <v>1.45038E-4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B94" s="5"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>46</v>
       </c>
@@ -3677,7 +3679,7 @@
         <v>1.008</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>112</v>
       </c>
@@ -3685,7 +3687,7 @@
         <v>4.0026020000000004</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>113</v>
       </c>
@@ -3693,7 +3695,7 @@
         <v>6.9379999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>114</v>
       </c>
@@ -3701,7 +3703,7 @@
         <v>9.0121830999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
         <v>115</v>
       </c>
@@ -3709,7 +3711,7 @@
         <v>10.805999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>38</v>
       </c>
@@ -3717,7 +3719,7 @@
         <v>12.0116</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>116</v>
       </c>
@@ -3725,7 +3727,7 @@
         <v>14.007</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>2</v>
       </c>
@@ -3733,7 +3735,7 @@
         <v>15.999000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>39</v>
       </c>
@@ -3741,7 +3743,7 @@
         <v>18.998403159999999</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>117</v>
       </c>
@@ -3749,7 +3751,7 @@
         <v>20.1797</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>5</v>
       </c>
@@ -3757,7 +3759,7 @@
         <v>22.989769280000001</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>118</v>
       </c>
@@ -3765,7 +3767,7 @@
         <v>24.305</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>119</v>
       </c>
@@ -3773,7 +3775,7 @@
         <v>26.981538499999999</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>120</v>
       </c>
@@ -3781,7 +3783,7 @@
         <v>28.085000000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>121</v>
       </c>
@@ -3789,7 +3791,7 @@
         <v>30.973762000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
         <v>122</v>
       </c>
@@ -3797,7 +3799,7 @@
         <v>32.06</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>123</v>
       </c>
@@ -3805,7 +3807,7 @@
         <v>35.450000000000003</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>124</v>
       </c>
@@ -3813,7 +3815,7 @@
         <v>39.948</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
         <v>37</v>
       </c>
@@ -3821,7 +3823,7 @@
         <v>39.098300000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
         <v>0</v>
       </c>
@@ -3829,7 +3831,7 @@
         <v>40.078000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
         <v>125</v>
       </c>
@@ -3837,7 +3839,7 @@
         <v>44.955908000000001</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>1</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>47.866999999999997</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>126</v>
       </c>
@@ -3853,7 +3855,7 @@
         <v>50.941499999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>127</v>
       </c>
@@ -3861,7 +3863,7 @@
         <v>51.996099999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>128</v>
       </c>
@@ -3869,7 +3871,7 @@
         <v>54.938043999999998</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>129</v>
       </c>
@@ -3877,7 +3879,7 @@
         <v>55.844999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>130</v>
       </c>
@@ -3885,7 +3887,7 @@
         <v>58.933194</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>131</v>
       </c>
@@ -3893,7 +3895,7 @@
         <v>58.693399999999997</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>132</v>
       </c>
@@ -3901,7 +3903,7 @@
         <v>63.545999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>133</v>
       </c>
@@ -3909,7 +3911,7 @@
         <v>65.38</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>134</v>
       </c>
@@ -3917,7 +3919,7 @@
         <v>69.722999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>135</v>
       </c>
@@ -3925,7 +3927,7 @@
         <v>72.63</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>136</v>
       </c>
@@ -3933,7 +3935,7 @@
         <v>74.921594999999996</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>137</v>
       </c>
@@ -3941,7 +3943,7 @@
         <v>78.971000000000004</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
         <v>138</v>
       </c>
@@ -3949,7 +3951,7 @@
         <v>79.900999999999996</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>139</v>
       </c>
@@ -3957,7 +3959,7 @@
         <v>83.798000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>140</v>
       </c>
@@ -3965,7 +3967,7 @@
         <v>85.467799999999997</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>141</v>
       </c>
@@ -3973,7 +3975,7 @@
         <v>87.62</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>142</v>
       </c>
@@ -3981,7 +3983,7 @@
         <v>88.905839999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>143</v>
       </c>
@@ -3989,7 +3991,7 @@
         <v>91.224000000000004</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>144</v>
       </c>
@@ -3997,7 +3999,7 @@
         <v>92.906369999999995</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>145</v>
       </c>
@@ -4005,7 +4007,7 @@
         <v>95.95</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
         <v>146</v>
       </c>
@@ -4013,7 +4015,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
         <v>147</v>
       </c>
@@ -4021,7 +4023,7 @@
         <v>101.07</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
         <v>148</v>
       </c>
@@ -4029,7 +4031,7 @@
         <v>102.9055</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
         <v>149</v>
       </c>
@@ -4037,7 +4039,7 @@
         <v>106.42</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
         <v>150</v>
       </c>
@@ -4045,7 +4047,7 @@
         <v>107.8682</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>151</v>
       </c>
@@ -4053,7 +4055,7 @@
         <v>112.414</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
         <v>152</v>
       </c>
@@ -4061,7 +4063,7 @@
         <v>114.818</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>153</v>
       </c>
@@ -4069,7 +4071,7 @@
         <v>118.71</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
         <v>154</v>
       </c>
@@ -4077,7 +4079,7 @@
         <v>121.76</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
         <v>155</v>
       </c>
@@ -4085,7 +4087,7 @@
         <v>127.6</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
         <v>156</v>
       </c>
@@ -4093,7 +4095,7 @@
         <v>126.90447</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
         <v>157</v>
       </c>
@@ -4101,7 +4103,7 @@
         <v>131.29300000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="6" t="s">
         <v>158</v>
       </c>
@@ -4109,7 +4111,7 @@
         <v>132.905452</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>159</v>
       </c>
@@ -4117,7 +4119,7 @@
         <v>137.327</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="6" t="s">
         <v>160</v>
       </c>
@@ -4125,7 +4127,7 @@
         <v>138.90547000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>161</v>
       </c>
@@ -4133,7 +4135,7 @@
         <v>140.11600000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="6" t="s">
         <v>162</v>
       </c>
@@ -4141,7 +4143,7 @@
         <v>140.90765999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
         <v>163</v>
       </c>
@@ -4149,7 +4151,7 @@
         <v>144.24199999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
         <v>164</v>
       </c>
@@ -4157,7 +4159,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
         <v>165</v>
       </c>
@@ -4165,7 +4167,7 @@
         <v>150.36000000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
         <v>166</v>
       </c>
@@ -4173,7 +4175,7 @@
         <v>151.964</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
         <v>167</v>
       </c>
@@ -4181,7 +4183,7 @@
         <v>157.25</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>168</v>
       </c>
@@ -4189,7 +4191,7 @@
         <v>158.92535000000001</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>169</v>
       </c>
@@ -4197,7 +4199,7 @@
         <v>162.5</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
         <v>170</v>
       </c>
@@ -4205,7 +4207,7 @@
         <v>164.93033</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="6" t="s">
         <v>171</v>
       </c>
@@ -4213,7 +4215,7 @@
         <v>167.25899999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
         <v>172</v>
       </c>
@@ -4221,7 +4223,7 @@
         <v>168.93422000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
         <v>173</v>
       </c>
@@ -4229,7 +4231,7 @@
         <v>173.054</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
         <v>174</v>
       </c>
@@ -4237,7 +4239,7 @@
         <v>174.96680000000001</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
         <v>175</v>
       </c>
@@ -4245,7 +4247,7 @@
         <v>178.49</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>176</v>
       </c>
@@ -4253,7 +4255,7 @@
         <v>180.94788</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>177</v>
       </c>
@@ -4261,7 +4263,7 @@
         <v>183.84</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="6" t="s">
         <v>178</v>
       </c>
@@ -4269,7 +4271,7 @@
         <v>186.20699999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
         <v>179</v>
       </c>
@@ -4277,7 +4279,7 @@
         <v>190.23</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
         <v>180</v>
       </c>
@@ -4285,7 +4287,7 @@
         <v>192.21700000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
         <v>181</v>
       </c>
@@ -4293,7 +4295,7 @@
         <v>195.084</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
         <v>182</v>
       </c>
@@ -4301,7 +4303,7 @@
         <v>196.96656899999999</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
         <v>183</v>
       </c>
@@ -4309,7 +4311,7 @@
         <v>200.59200000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>184</v>
       </c>
@@ -4317,7 +4319,7 @@
         <v>204.38200000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>185</v>
       </c>
@@ -4325,7 +4327,7 @@
         <v>207.2</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
         <v>186</v>
       </c>
@@ -4333,7 +4335,7 @@
         <v>208.9804</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
         <v>187</v>
       </c>
@@ -4341,7 +4343,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
         <v>188</v>
       </c>
@@ -4349,7 +4351,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="6" t="s">
         <v>189</v>
       </c>
@@ -4357,7 +4359,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="6" t="s">
         <v>190</v>
       </c>
@@ -4365,7 +4367,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="6" t="s">
         <v>191</v>
       </c>
@@ -4373,7 +4375,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>192</v>
       </c>
@@ -4381,7 +4383,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
         <v>193</v>
       </c>
@@ -4389,7 +4391,7 @@
         <v>232.0377</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
         <v>12</v>
       </c>
@@ -4397,7 +4399,7 @@
         <v>231.03587999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="6" t="s">
         <v>194</v>
       </c>
@@ -4405,7 +4407,7 @@
         <v>238.02891</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="6" t="s">
         <v>195</v>
       </c>
@@ -4413,7 +4415,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="6" t="s">
         <v>196</v>
       </c>
@@ -4421,7 +4423,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
         <v>197</v>
       </c>
@@ -4429,7 +4431,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="6" t="s">
         <v>198</v>
       </c>
@@ -4437,7 +4439,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="6" t="s">
         <v>199</v>
       </c>
@@ -4445,7 +4447,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
         <v>200</v>
       </c>
@@ -4453,7 +4455,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
         <v>201</v>
       </c>
@@ -4461,7 +4463,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="6" t="s">
         <v>202</v>
       </c>
@@ -4469,7 +4471,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
         <v>203</v>
       </c>
@@ -4477,7 +4479,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
         <v>204</v>
       </c>
@@ -4485,7 +4487,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="6" t="s">
         <v>205</v>
       </c>
@@ -4493,7 +4495,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
         <v>206</v>
       </c>
@@ -4501,7 +4503,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
         <v>207</v>
       </c>
@@ -4509,7 +4511,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="6" t="s">
         <v>208</v>
       </c>
@@ -4517,7 +4519,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="6" t="s">
         <v>209</v>
       </c>
@@ -4525,7 +4527,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
         <v>210</v>
       </c>
@@ -4533,7 +4535,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
         <v>211</v>
       </c>
@@ -4541,7 +4543,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
         <v>212</v>
       </c>
@@ -4549,7 +4551,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="6" t="s">
         <v>213</v>
       </c>
@@ -4557,7 +4559,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="6" t="s">
         <v>214</v>
       </c>
@@ -4565,7 +4567,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="6" t="s">
         <v>215</v>
       </c>
@@ -4573,7 +4575,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="6" t="s">
         <v>216</v>
       </c>
@@ -4581,7 +4583,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="6" t="s">
         <v>217</v>
       </c>
@@ -4589,7 +4591,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="6" t="s">
         <v>218</v>
       </c>
@@ -4597,7 +4599,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A211" s="9" t="s">
         <v>219</v>
       </c>

</xml_diff>

<commit_message>
Fix Unit Test issues
</commit_message>
<xml_diff>
--- a/pmutt/tests/test_constants.xlsx
+++ b/pmutt/tests/test_constants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerhard\Documents\GitHub\pMuTT\pmutt\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1352783B-40D7-4FC2-94A5-057F9145BCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95987D48-EB17-4DA6-A9A2-DDE7EEC09286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="0" windowWidth="28710" windowHeight="15480" activeTab="1" xr2:uid="{AA336A12-CD5D-469F-9132-8EBAE81227A9}"/>
+    <workbookView xWindow="90" yWindow="0" windowWidth="28710" windowHeight="15480" activeTab="2" xr2:uid="{AA336A12-CD5D-469F-9132-8EBAE81227A9}"/>
   </bookViews>
   <sheets>
     <sheet name="ans" sheetId="3" r:id="rId1"/>
@@ -938,8 +938,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000000000000"/>
-    <numFmt numFmtId="172" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1112,9 +1112,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Input" xfId="1" builtinId="20" customBuiltin="1"/>
@@ -1818,7 +1818,7 @@
       </c>
       <c r="B12" s="2">
         <f>test_constants!B22</f>
-        <v>24177991103754.523</v>
+        <v>24179892822261.859</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="B13" s="2">
         <f>test_constants!B26</f>
-        <v>1160.3609474768741</v>
+        <v>1160.4522156008277</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1836,7 +1836,7 @@
       </c>
       <c r="B14" s="2">
         <f>test_constants!B30</f>
-        <v>806.49097262328473</v>
+        <v>806.55440712460688</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B15" s="2">
         <f>test_constants!B34*constants!B15/constants!B17</f>
-        <v>2.5689025147068248E-39</v>
+        <v>2.5691045715871832E-39</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="B18" s="2">
         <f>test_constants!B46</f>
-        <v>0.55933568955994584</v>
+        <v>0.55937968407661531</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1965,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E805CA-ACAA-4599-A8B2-1C6F37F3FD7A}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="B22" s="10">
         <f>B21*constants!B15/constants!B17/h_Js</f>
-        <v>24177991103754.523</v>
+        <v>24179892822261.859</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>103</v>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="B26" s="10">
         <f>B21*constants!B15/constants!B17/kb_JK</f>
-        <v>1160.3609474768741</v>
+        <v>1160.4522156008277</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>37</v>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B30" s="10">
         <f>B21*constants!B15/constants!B17/h_Js/c_cms</f>
-        <v>806.49097262328473</v>
+        <v>806.55440712460688</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>108</v>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="B46" s="10">
         <f>(h_eVs/2/PI())^2/2/kb_eVK/B45/constants!B17</f>
-        <v>0.55933568955994584</v>
+        <v>0.55937968407661531</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>37</v>
@@ -2619,7 +2619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2E394F-E007-4BF1-81D0-B5B598FFC5B9}">
   <dimension ref="A1:AH211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3129,7 +3129,7 @@
         <v>101</v>
       </c>
       <c r="B17" s="2">
-        <v>6.242E+18</v>
+        <v>6.2415090744607498E+18</v>
       </c>
       <c r="H17" s="24"/>
     </row>

</xml_diff>